<commit_message>
feat: código semana 4
</commit_message>
<xml_diff>
--- a/alunos.xlsx
+++ b/alunos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia\Documents\Letícia\Repositórios\latelie_de_verao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFDDC0A-6BD5-4BC7-9D43-AC2EFAA9F0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E8F88E-082D-4F65-B7BE-15724AB0FE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5BD735D1-F3B0-4DC0-AB17-30AB545D3AA1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="386">
   <si>
     <t xml:space="preserve">Nome completo
 </t>
@@ -1189,6 +1189,12 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1buDrBqk4rHcGLbKKMJHOEOM9AOosdrVF</t>
+  </si>
+  <si>
+    <t>Atividade 3</t>
+  </si>
+  <si>
+    <t>Qntd. de Palavras Atv. 3</t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1540,7 +1546,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1559,9 +1564,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1574,9 +1576,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1585,6 +1584,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1921,32 +1924,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C2AB94-8371-415B-B15C-673BF998D579}">
-  <dimension ref="A1:R54"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="134.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.77734375" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="66.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="66.21875" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="65" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.77734375" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="22" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="35.77734375" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="134.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.77734375" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="66.88671875" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="66.21875" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="65" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.77734375" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="22" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.88671875" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1989,21 +1992,27 @@
       <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="14" t="s">
         <v>379</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2039,27 +2048,33 @@
       <c r="L2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q2" s="4">
         <v>207</v>
       </c>
-      <c r="Q2" s="19">
+      <c r="R2" s="18">
         <v>0</v>
       </c>
-      <c r="R2" s="19">
+      <c r="S2" s="18">
+        <v>0</v>
+      </c>
+      <c r="T2" s="18">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2095,27 +2110,33 @@
       <c r="L3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P3" s="7">
+      <c r="O3" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q3" s="7">
         <v>645</v>
       </c>
-      <c r="Q3" s="22">
+      <c r="R3" s="21">
         <v>1170</v>
       </c>
-      <c r="R3" s="22">
-        <v>1815</v>
+      <c r="S3" s="21">
+        <v>376</v>
+      </c>
+      <c r="T3" s="21">
+        <v>2191</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2151,27 +2172,33 @@
       <c r="L4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P4" s="4">
+      <c r="O4" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q4" s="4">
         <v>243</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="R4" s="18">
         <v>358</v>
       </c>
-      <c r="R4" s="19">
+      <c r="S4" s="18">
+        <v>0</v>
+      </c>
+      <c r="T4" s="18">
         <v>601</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2207,27 +2234,33 @@
       <c r="L5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P5" s="7">
+      <c r="O5" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P5" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q5" s="7">
         <v>1992</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="R5" s="21">
         <v>3976</v>
       </c>
-      <c r="R5" s="22">
-        <v>5968</v>
+      <c r="S5" s="21">
+        <v>2344</v>
+      </c>
+      <c r="T5" s="21">
+        <v>8312</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2263,27 +2296,33 @@
       <c r="L6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P6" s="4">
+      <c r="O6" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q6" s="4">
         <v>1870</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="R6" s="18">
         <v>1383</v>
       </c>
-      <c r="R6" s="19">
-        <v>3253</v>
+      <c r="S6" s="18">
+        <v>495</v>
+      </c>
+      <c r="T6" s="18">
+        <v>3748</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2319,27 +2358,33 @@
       <c r="L7" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P7" s="7">
+      <c r="O7" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q7" s="7">
         <v>514</v>
       </c>
-      <c r="Q7" s="22">
+      <c r="R7" s="21">
         <v>868</v>
       </c>
-      <c r="R7" s="22">
-        <v>1382</v>
+      <c r="S7" s="21">
+        <v>86</v>
+      </c>
+      <c r="T7" s="21">
+        <v>1468</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
         <v>68</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2375,27 +2420,33 @@
       <c r="L8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P8" s="4">
+      <c r="O8" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q8" s="4">
         <v>269</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="R8" s="18">
         <v>474</v>
       </c>
-      <c r="R8" s="19">
-        <v>743</v>
+      <c r="S8" s="18">
+        <v>320</v>
+      </c>
+      <c r="T8" s="18">
+        <v>1063</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
         <v>75</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2431,27 +2482,33 @@
       <c r="L9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="M9" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P9" s="7">
+      <c r="O9" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q9" s="7">
         <v>261</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="R9" s="21">
         <v>766</v>
       </c>
-      <c r="R9" s="22">
-        <v>1027</v>
+      <c r="S9" s="21">
+        <v>478</v>
+      </c>
+      <c r="T9" s="21">
+        <v>1505</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2487,27 +2544,33 @@
       <c r="L10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P10" s="4">
+      <c r="O10" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P10" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q10" s="4">
         <v>355</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="R10" s="18">
         <v>868</v>
       </c>
-      <c r="R10" s="19">
-        <v>1223</v>
+      <c r="S10" s="18">
+        <v>420</v>
+      </c>
+      <c r="T10" s="18">
+        <v>1643</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
         <v>91</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -2543,27 +2606,33 @@
       <c r="L11" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="M11" s="21" t="s">
+      <c r="M11" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O11" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P11" s="7">
+      <c r="O11" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q11" s="7">
         <v>549</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="R11" s="21">
         <v>3324</v>
       </c>
-      <c r="R11" s="22">
-        <v>3873</v>
+      <c r="S11" s="21">
+        <v>1745</v>
+      </c>
+      <c r="T11" s="21">
+        <v>5618</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="16" t="s">
         <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2599,27 +2668,33 @@
       <c r="L12" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M12" s="18" t="s">
+      <c r="M12" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="18" t="s">
+      <c r="O12" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q12" s="4">
         <v>789</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="R12" s="18">
         <v>0</v>
       </c>
-      <c r="R12" s="19">
+      <c r="S12" s="18">
+        <v>0</v>
+      </c>
+      <c r="T12" s="18">
         <v>789</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
         <v>105</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2655,27 +2730,33 @@
       <c r="L13" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="M13" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P13" s="7">
+      <c r="O13" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q13" s="7">
         <v>783</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="R13" s="21">
         <v>1466</v>
       </c>
-      <c r="R13" s="22">
-        <v>2249</v>
+      <c r="S13" s="21">
+        <v>741</v>
+      </c>
+      <c r="T13" s="21">
+        <v>2990</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
         <v>112</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2711,27 +2792,33 @@
       <c r="L14" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="M14" s="18" t="s">
+      <c r="M14" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P14" s="4">
+      <c r="O14" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P14" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q14" s="4">
         <v>565</v>
       </c>
-      <c r="Q14" s="19">
+      <c r="R14" s="18">
         <v>884</v>
       </c>
-      <c r="R14" s="19">
+      <c r="S14" s="18">
+        <v>0</v>
+      </c>
+      <c r="T14" s="18">
         <v>1449</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="19" t="s">
         <v>121</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -2767,27 +2854,33 @@
       <c r="L15" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="M15" s="21" t="s">
+      <c r="M15" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P15" s="7">
+      <c r="O15" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P15" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q15" s="7">
         <v>394</v>
       </c>
-      <c r="Q15" s="22">
+      <c r="R15" s="21">
         <v>1845</v>
       </c>
-      <c r="R15" s="22">
-        <v>2239</v>
+      <c r="S15" s="21">
+        <v>1041</v>
+      </c>
+      <c r="T15" s="21">
+        <v>3280</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="s">
         <v>127</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2823,27 +2916,33 @@
       <c r="L16" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="M16" s="18" t="s">
+      <c r="M16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O16" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P16" s="4">
+      <c r="O16" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P16" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q16" s="4">
         <v>1935</v>
       </c>
-      <c r="Q16" s="19">
+      <c r="R16" s="18">
         <v>1620</v>
       </c>
-      <c r="R16" s="19">
-        <v>3555</v>
+      <c r="S16" s="18">
+        <v>759</v>
+      </c>
+      <c r="T16" s="18">
+        <v>4314</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
+    <row r="17" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="19" t="s">
         <v>133</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -2879,27 +2978,33 @@
       <c r="L17" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="M17" s="21" t="s">
+      <c r="M17" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O17" s="21" t="s">
+      <c r="O17" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q17" s="7">
         <v>683</v>
       </c>
-      <c r="Q17" s="22">
+      <c r="R17" s="21">
         <v>0</v>
       </c>
-      <c r="R17" s="22">
+      <c r="S17" s="21">
+        <v>0</v>
+      </c>
+      <c r="T17" s="21">
         <v>683</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="16" t="s">
         <v>140</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2935,27 +3040,33 @@
       <c r="L18" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="M18" s="18" t="s">
+      <c r="M18" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O18" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P18" s="4">
+      <c r="O18" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P18" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q18" s="4">
         <v>908</v>
       </c>
-      <c r="Q18" s="19">
+      <c r="R18" s="18">
         <v>1612</v>
       </c>
-      <c r="R18" s="19">
-        <v>2520</v>
+      <c r="S18" s="18">
+        <v>681</v>
+      </c>
+      <c r="T18" s="18">
+        <v>3201</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="19" t="s">
         <v>147</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -2991,27 +3102,33 @@
       <c r="L19" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="M19" s="21" t="s">
+      <c r="M19" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O19" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P19" s="7">
+      <c r="O19" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P19" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q19" s="7">
         <v>818</v>
       </c>
-      <c r="Q19" s="22">
+      <c r="R19" s="21">
         <v>1226</v>
       </c>
-      <c r="R19" s="22">
+      <c r="S19" s="21">
+        <v>0</v>
+      </c>
+      <c r="T19" s="21">
         <v>2044</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="16" t="s">
         <v>154</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -3047,27 +3164,33 @@
       <c r="L20" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="M20" s="18" t="s">
+      <c r="M20" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P20" s="4">
+      <c r="O20" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P20" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q20" s="4">
         <v>720</v>
       </c>
-      <c r="Q20" s="19">
+      <c r="R20" s="18">
         <v>1177</v>
       </c>
-      <c r="R20" s="19">
-        <v>1897</v>
+      <c r="S20" s="18">
+        <v>1256</v>
+      </c>
+      <c r="T20" s="18">
+        <v>3153</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="19" t="s">
         <v>161</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -3103,27 +3226,33 @@
       <c r="L21" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="M21" s="21" t="s">
+      <c r="M21" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N21" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O21" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P21" s="7">
+      <c r="O21" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P21" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q21" s="7">
         <v>964</v>
       </c>
-      <c r="Q21" s="22">
+      <c r="R21" s="21">
         <v>575</v>
       </c>
-      <c r="R21" s="22">
-        <v>1539</v>
+      <c r="S21" s="21">
+        <v>760</v>
+      </c>
+      <c r="T21" s="21">
+        <v>2299</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
         <v>167</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -3159,27 +3288,33 @@
       <c r="L22" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="M22" s="18" t="s">
+      <c r="M22" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P22" s="4">
+      <c r="O22" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P22" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q22" s="4">
         <v>5001</v>
       </c>
-      <c r="Q22" s="19">
+      <c r="R22" s="18">
         <v>7230</v>
       </c>
-      <c r="R22" s="19">
-        <v>12231</v>
+      <c r="S22" s="18">
+        <v>5756</v>
+      </c>
+      <c r="T22" s="18">
+        <v>17987</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
+    <row r="23" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
         <v>174</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -3215,27 +3350,33 @@
       <c r="L23" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="M23" s="21" t="s">
+      <c r="M23" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O23" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P23" s="7">
+      <c r="O23" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P23" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q23" s="7">
         <v>490</v>
       </c>
-      <c r="Q23" s="22">
+      <c r="R23" s="21">
         <v>696</v>
       </c>
-      <c r="R23" s="22">
-        <v>1186</v>
+      <c r="S23" s="21">
+        <v>245</v>
+      </c>
+      <c r="T23" s="21">
+        <v>1431</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
         <v>180</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -3271,25 +3412,33 @@
       <c r="L24" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M24" s="18" t="s">
+      <c r="M24" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O24" s="18" t="s">
+      <c r="O24" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P24" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q24" s="4">
         <v>446</v>
       </c>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="19">
+      <c r="R24" s="18">
+        <v>0</v>
+      </c>
+      <c r="S24" s="18">
+        <v>0</v>
+      </c>
+      <c r="T24" s="18">
         <v>446</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
+    <row r="25" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="19" t="s">
         <v>187</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -3325,25 +3474,33 @@
       <c r="L25" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="M25" s="21" t="s">
+      <c r="M25" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O25" s="21" t="s">
+      <c r="O25" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q25" s="7">
         <v>543</v>
       </c>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="22">
+      <c r="R25" s="21">
+        <v>0</v>
+      </c>
+      <c r="S25" s="21">
+        <v>0</v>
+      </c>
+      <c r="T25" s="21">
         <v>543</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="16" t="s">
         <v>192</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -3379,27 +3536,33 @@
       <c r="L26" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="M26" s="18" t="s">
+      <c r="M26" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O26" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P26" s="4">
+      <c r="O26" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q26" s="4">
         <v>1145</v>
       </c>
-      <c r="Q26" s="19">
+      <c r="R26" s="18">
         <v>1820</v>
       </c>
-      <c r="R26" s="19">
-        <v>2965</v>
+      <c r="S26" s="18">
+        <v>1340</v>
+      </c>
+      <c r="T26" s="18">
+        <v>4305</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="20" t="s">
+    <row r="27" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="19" t="s">
         <v>198</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -3435,27 +3598,33 @@
       <c r="L27" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="M27" s="21" t="s">
+      <c r="M27" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N27" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O27" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P27" s="7">
+      <c r="O27" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P27" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q27" s="7">
         <v>607</v>
       </c>
-      <c r="Q27" s="22">
+      <c r="R27" s="21">
         <v>808</v>
       </c>
-      <c r="R27" s="22">
-        <v>1415</v>
+      <c r="S27" s="21">
+        <v>778</v>
+      </c>
+      <c r="T27" s="21">
+        <v>2193</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="17" t="s">
+    <row r="28" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="16" t="s">
         <v>204</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3491,27 +3660,33 @@
       <c r="L28" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="M28" s="18" t="s">
+      <c r="M28" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O28" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P28" s="4">
+      <c r="O28" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q28" s="4">
         <v>555</v>
       </c>
-      <c r="Q28" s="19">
+      <c r="R28" s="18">
         <v>445</v>
       </c>
-      <c r="R28" s="19">
+      <c r="S28" s="18">
+        <v>0</v>
+      </c>
+      <c r="T28" s="18">
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
+    <row r="29" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="19" t="s">
         <v>210</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -3547,27 +3722,33 @@
       <c r="L29" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="M29" s="21" t="s">
+      <c r="M29" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N29" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="O29" s="21" t="s">
+      <c r="O29" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="P29" s="7">
+      <c r="P29" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q29" s="7">
         <v>0</v>
       </c>
-      <c r="Q29" s="22">
+      <c r="R29" s="21">
         <v>0</v>
       </c>
-      <c r="R29" s="22">
+      <c r="S29" s="21">
         <v>0</v>
       </c>
+      <c r="T29" s="21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="17" t="s">
+    <row r="30" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="16" t="s">
         <v>217</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3603,27 +3784,33 @@
       <c r="L30" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="M30" s="18" t="s">
+      <c r="M30" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="O30" s="18" t="s">
+      <c r="O30" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="P30" s="4">
+      <c r="P30" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q30" s="4">
         <v>0</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="R30" s="18">
         <v>0</v>
       </c>
-      <c r="R30" s="19">
+      <c r="S30" s="18">
         <v>0</v>
       </c>
+      <c r="T30" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="20" t="s">
+    <row r="31" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="19" t="s">
         <v>223</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -3659,27 +3846,33 @@
       <c r="L31" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="M31" s="21" t="s">
+      <c r="M31" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N31" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O31" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P31" s="7">
+      <c r="O31" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P31" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q31" s="7">
         <v>514</v>
       </c>
-      <c r="Q31" s="22">
+      <c r="R31" s="21">
         <v>1382</v>
       </c>
-      <c r="R31" s="22">
-        <v>1896</v>
+      <c r="S31" s="21">
+        <v>1343</v>
+      </c>
+      <c r="T31" s="21">
+        <v>3239</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="17" t="s">
+    <row r="32" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="16" t="s">
         <v>229</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3715,27 +3908,33 @@
       <c r="L32" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="M32" s="18" t="s">
+      <c r="M32" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O32" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P32" s="4">
+      <c r="O32" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P32" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q32" s="4">
         <v>2234</v>
       </c>
-      <c r="Q32" s="19">
+      <c r="R32" s="18">
         <v>3447</v>
       </c>
-      <c r="R32" s="19">
-        <v>5681</v>
+      <c r="S32" s="18">
+        <v>1127</v>
+      </c>
+      <c r="T32" s="18">
+        <v>6808</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="20" t="s">
+    <row r="33" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="19" t="s">
         <v>237</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -3771,27 +3970,33 @@
       <c r="L33" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="M33" s="21" t="s">
+      <c r="M33" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O33" s="21" t="s">
+      <c r="O33" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="P33" s="7">
+      <c r="P33" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q33" s="7">
         <v>407</v>
       </c>
-      <c r="Q33" s="22">
+      <c r="R33" s="21">
         <v>0</v>
       </c>
-      <c r="R33" s="22">
-        <v>407</v>
+      <c r="S33" s="21">
+        <v>761</v>
+      </c>
+      <c r="T33" s="21">
+        <v>1168</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="17" t="s">
+    <row r="34" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="16" t="s">
         <v>243</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -3827,27 +4032,33 @@
       <c r="L34" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="M34" s="18" t="s">
+      <c r="M34" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O34" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P34" s="4">
+      <c r="O34" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P34" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q34" s="4">
         <v>462</v>
       </c>
-      <c r="Q34" s="19">
+      <c r="R34" s="18">
         <v>978</v>
       </c>
-      <c r="R34" s="19">
-        <v>1440</v>
+      <c r="S34" s="18">
+        <v>1281</v>
+      </c>
+      <c r="T34" s="18">
+        <v>2721</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="20" t="s">
+    <row r="35" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="19" t="s">
         <v>250</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -3883,27 +4094,33 @@
       <c r="L35" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="M35" s="21" t="s">
+      <c r="M35" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N35" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O35" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P35" s="7">
+      <c r="O35" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P35" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q35" s="7">
         <v>658</v>
       </c>
-      <c r="Q35" s="22">
+      <c r="R35" s="21">
         <v>709</v>
       </c>
-      <c r="R35" s="22">
-        <v>1367</v>
+      <c r="S35" s="21">
+        <v>818</v>
+      </c>
+      <c r="T35" s="21">
+        <v>2185</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="17" t="s">
+    <row r="36" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="16" t="s">
         <v>256</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3939,27 +4156,33 @@
       <c r="L36" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="M36" s="18" t="s">
+      <c r="M36" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O36" s="18" t="s">
+      <c r="O36" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="P36" s="4">
+      <c r="P36" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q36" s="4">
         <v>1350</v>
       </c>
-      <c r="Q36" s="19">
+      <c r="R36" s="18">
         <v>0</v>
       </c>
-      <c r="R36" s="19">
+      <c r="S36" s="18">
+        <v>0</v>
+      </c>
+      <c r="T36" s="18">
         <v>1350</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="19" t="s">
         <v>263</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -3995,27 +4218,33 @@
       <c r="L37" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="M37" s="21" t="s">
+      <c r="M37" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N37" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O37" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P37" s="7">
+      <c r="O37" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P37" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q37" s="7">
         <v>2381</v>
       </c>
-      <c r="Q37" s="22">
+      <c r="R37" s="21">
         <v>1268</v>
       </c>
-      <c r="R37" s="22">
+      <c r="S37" s="21">
+        <v>0</v>
+      </c>
+      <c r="T37" s="21">
         <v>3649</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="17" t="s">
+    <row r="38" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="16" t="s">
         <v>270</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -4051,27 +4280,33 @@
       <c r="L38" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="M38" s="18" t="s">
+      <c r="M38" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O38" s="18" t="s">
+      <c r="O38" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="P38" s="4">
+      <c r="P38" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q38" s="4">
         <v>1293</v>
       </c>
-      <c r="Q38" s="19">
+      <c r="R38" s="18">
         <v>0</v>
       </c>
-      <c r="R38" s="19">
+      <c r="S38" s="18">
+        <v>0</v>
+      </c>
+      <c r="T38" s="18">
         <v>1293</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="20" t="s">
+    <row r="39" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="19" t="s">
         <v>276</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -4107,27 +4342,33 @@
       <c r="L39" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="M39" s="21" t="s">
+      <c r="M39" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N39" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O39" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P39" s="7">
+      <c r="O39" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P39" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q39" s="7">
         <v>590</v>
       </c>
-      <c r="Q39" s="22">
+      <c r="R39" s="21">
         <v>4626</v>
       </c>
-      <c r="R39" s="22">
+      <c r="S39" s="21">
+        <v>0</v>
+      </c>
+      <c r="T39" s="21">
         <v>5216</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="17" t="s">
+    <row r="40" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="16" t="s">
         <v>282</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -4163,27 +4404,33 @@
       <c r="L40" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="M40" s="18" t="s">
+      <c r="M40" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O40" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P40" s="4">
+      <c r="O40" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P40" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q40" s="4">
         <v>2176</v>
       </c>
-      <c r="Q40" s="19">
+      <c r="R40" s="18">
         <v>3627</v>
       </c>
-      <c r="R40" s="19">
-        <v>5803</v>
+      <c r="S40" s="18">
+        <v>1653</v>
+      </c>
+      <c r="T40" s="18">
+        <v>7456</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="20" t="s">
+    <row r="41" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="19" t="s">
         <v>289</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -4219,27 +4466,33 @@
       <c r="L41" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="M41" s="21" t="s">
+      <c r="M41" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N41" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O41" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P41" s="7">
+      <c r="O41" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P41" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q41" s="7">
         <v>524</v>
       </c>
-      <c r="Q41" s="22">
+      <c r="R41" s="21">
         <v>1259</v>
       </c>
-      <c r="R41" s="22">
-        <v>1783</v>
+      <c r="S41" s="21">
+        <v>1212</v>
+      </c>
+      <c r="T41" s="21">
+        <v>2995</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="17" t="s">
+    <row r="42" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="16" t="s">
         <v>295</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -4273,27 +4526,33 @@
         <v>26</v>
       </c>
       <c r="L42" s="8"/>
-      <c r="M42" s="18" t="s">
+      <c r="M42" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N42" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O42" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P42" s="4">
+      <c r="O42" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P42" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q42" s="4">
         <v>2080</v>
       </c>
-      <c r="Q42" s="19">
+      <c r="R42" s="18">
         <v>1638</v>
       </c>
-      <c r="R42" s="19">
-        <v>3718</v>
+      <c r="S42" s="18">
+        <v>779</v>
+      </c>
+      <c r="T42" s="18">
+        <v>4497</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="20" t="s">
+    <row r="43" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="19" t="s">
         <v>300</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -4329,27 +4588,33 @@
       <c r="L43" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="M43" s="21" t="s">
+      <c r="M43" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N43" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O43" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P43" s="7">
+      <c r="O43" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P43" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q43" s="7">
         <v>1716</v>
       </c>
-      <c r="Q43" s="22">
+      <c r="R43" s="21">
         <v>2216</v>
       </c>
-      <c r="R43" s="22">
-        <v>3932</v>
+      <c r="S43" s="21">
+        <v>842</v>
+      </c>
+      <c r="T43" s="21">
+        <v>4774</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="17" t="s">
+    <row r="44" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="16" t="s">
         <v>306</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -4385,27 +4650,33 @@
       <c r="L44" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="M44" s="18" t="s">
+      <c r="M44" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="O44" s="18" t="s">
+      <c r="O44" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="P44" s="4">
+      <c r="P44" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q44" s="4">
         <v>0</v>
       </c>
-      <c r="Q44" s="19">
+      <c r="R44" s="18">
         <v>0</v>
       </c>
-      <c r="R44" s="19">
+      <c r="S44" s="18">
         <v>0</v>
       </c>
+      <c r="T44" s="18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="20" t="s">
+    <row r="45" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="19" t="s">
         <v>312</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -4441,27 +4712,33 @@
       <c r="L45" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="M45" s="21" t="s">
+      <c r="M45" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N45" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O45" s="21" t="s">
+      <c r="O45" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="P45" s="7">
+      <c r="P45" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q45" s="7">
         <v>787</v>
       </c>
-      <c r="Q45" s="22">
+      <c r="R45" s="21">
         <v>0</v>
       </c>
-      <c r="R45" s="22">
-        <v>787</v>
+      <c r="S45" s="21">
+        <v>815</v>
+      </c>
+      <c r="T45" s="21">
+        <v>1602</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="17" t="s">
+    <row r="46" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="16" t="s">
         <v>319</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -4497,27 +4774,33 @@
       <c r="L46" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="M46" s="18" t="s">
+      <c r="M46" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N46" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O46" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P46" s="4">
+      <c r="O46" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P46" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q46" s="4">
         <v>268</v>
       </c>
-      <c r="Q46" s="19">
+      <c r="R46" s="18">
         <v>507</v>
       </c>
-      <c r="R46" s="19">
-        <v>775</v>
+      <c r="S46" s="18">
+        <v>603</v>
+      </c>
+      <c r="T46" s="18">
+        <v>1378</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="20" t="s">
+    <row r="47" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="19" t="s">
         <v>326</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -4553,27 +4836,33 @@
       <c r="L47" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="M47" s="21" t="s">
+      <c r="M47" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N47" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O47" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P47" s="7">
+      <c r="O47" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P47" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q47" s="7">
         <v>633</v>
       </c>
-      <c r="Q47" s="22">
+      <c r="R47" s="21">
         <v>4260</v>
       </c>
-      <c r="R47" s="22">
-        <v>4893</v>
+      <c r="S47" s="21">
+        <v>552</v>
+      </c>
+      <c r="T47" s="21">
+        <v>5445</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="17" t="s">
+    <row r="48" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="16" t="s">
         <v>332</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -4609,27 +4898,33 @@
       <c r="L48" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="M48" s="18" t="s">
+      <c r="M48" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O48" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P48" s="4">
+      <c r="O48" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P48" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q48" s="4">
         <v>1755</v>
       </c>
-      <c r="Q48" s="19">
+      <c r="R48" s="18">
         <v>3189</v>
       </c>
-      <c r="R48" s="19">
-        <v>4944</v>
+      <c r="S48" s="18">
+        <v>3735</v>
+      </c>
+      <c r="T48" s="18">
+        <v>8679</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="20" t="s">
+    <row r="49" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="19" t="s">
         <v>339</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -4665,27 +4960,33 @@
       <c r="L49" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="M49" s="21" t="s">
+      <c r="M49" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N49" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O49" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P49" s="7">
+      <c r="O49" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P49" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q49" s="7">
         <v>424</v>
       </c>
-      <c r="Q49" s="22">
+      <c r="R49" s="21">
         <v>3217</v>
       </c>
-      <c r="R49" s="22">
-        <v>3641</v>
+      <c r="S49" s="21">
+        <v>253</v>
+      </c>
+      <c r="T49" s="21">
+        <v>3894</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="17" t="s">
+    <row r="50" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="16" t="s">
         <v>346</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -4721,27 +5022,33 @@
       <c r="L50" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="M50" s="18" t="s">
+      <c r="M50" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O50" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P50" s="4">
+      <c r="O50" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P50" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q50" s="4">
         <v>522</v>
       </c>
-      <c r="Q50" s="19">
+      <c r="R50" s="18">
         <v>2749</v>
       </c>
-      <c r="R50" s="19">
-        <v>3271</v>
+      <c r="S50" s="18">
+        <v>754</v>
+      </c>
+      <c r="T50" s="18">
+        <v>4025</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="20" t="s">
+    <row r="51" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="19" t="s">
         <v>352</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -4777,27 +5084,33 @@
       <c r="L51" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="M51" s="21" t="s">
+      <c r="M51" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N51" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O51" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P51" s="7">
+      <c r="O51" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P51" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q51" s="7">
         <v>1408</v>
       </c>
-      <c r="Q51" s="22">
+      <c r="R51" s="21">
         <v>1052</v>
       </c>
-      <c r="R51" s="22">
-        <v>2460</v>
+      <c r="S51" s="21">
+        <v>906</v>
+      </c>
+      <c r="T51" s="21">
+        <v>3366</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="17" t="s">
+    <row r="52" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="16" t="s">
         <v>359</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -4833,27 +5146,33 @@
       <c r="L52" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="M52" s="18" t="s">
+      <c r="M52" s="17" t="s">
         <v>28</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O52" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="P52" s="4">
+      <c r="O52" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="P52" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q52" s="4">
         <v>662</v>
       </c>
-      <c r="Q52" s="19">
+      <c r="R52" s="18">
         <v>643</v>
       </c>
-      <c r="R52" s="19">
-        <v>1305</v>
+      <c r="S52" s="18">
+        <v>373</v>
+      </c>
+      <c r="T52" s="18">
+        <v>1678</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="20" t="s">
+    <row r="53" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="19" t="s">
         <v>366</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -4889,27 +5208,31 @@
       <c r="L53" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="M53" s="21" t="s">
+      <c r="M53" s="20" t="s">
         <v>28</v>
       </c>
       <c r="N53" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O53" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="P53" s="7">
+      <c r="O53" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="P53" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q53" s="7">
         <v>684</v>
       </c>
-      <c r="Q53" s="22">
+      <c r="R53" s="21">
         <v>1573</v>
       </c>
-      <c r="R53" s="22">
+      <c r="S53" s="22"/>
+      <c r="T53" s="21">
         <v>2257</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="25" t="s">
+    <row r="54" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="23" t="s">
         <v>373</v>
       </c>
       <c r="B54" s="9" t="s">
@@ -4931,129 +5254,135 @@
       <c r="J54" s="10"/>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
-      <c r="M54" s="26"/>
-      <c r="N54" s="27" t="s">
+      <c r="M54" s="24"/>
+      <c r="N54" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="O54" s="28" t="s">
+      <c r="O54" s="25" t="s">
         <v>381</v>
       </c>
-      <c r="P54" s="29">
+      <c r="P54" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q54" s="26">
         <v>0</v>
       </c>
-      <c r="Q54" s="30">
+      <c r="R54" s="27">
         <v>0</v>
       </c>
-      <c r="R54" s="31">
+      <c r="S54" s="28">
+        <v>0</v>
+      </c>
+      <c r="T54" s="28">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{EB738A8F-B3AC-4F21-9ECF-BFEA8B187D24}"/>
-    <hyperlink ref="L2" r:id="rId2" xr:uid="{E3503D9E-C635-429A-B842-A9FB43547436}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{EE968E23-0BBA-408A-8F73-A473B9EA86F2}"/>
-    <hyperlink ref="L3" r:id="rId4" xr:uid="{F28C4BA9-FF70-4617-8ADC-F018E8DBD3B3}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{4F654CFC-8F81-472B-AD41-78CF5F0370FD}"/>
-    <hyperlink ref="L4" r:id="rId6" xr:uid="{E331795C-E17E-4C0F-9DC2-7372D547B6DF}"/>
-    <hyperlink ref="F5" r:id="rId7" xr:uid="{04E2D06C-8BFE-488E-9B4C-B3C68A724C2E}"/>
-    <hyperlink ref="L5" r:id="rId8" xr:uid="{EEEAA601-FFA7-4972-BE77-BD271A7604D9}"/>
-    <hyperlink ref="F6" r:id="rId9" xr:uid="{37660679-92C2-4865-998D-A0D3B6EF2B7F}"/>
-    <hyperlink ref="L6" r:id="rId10" xr:uid="{2122171C-4648-4719-9257-C5A460D54B49}"/>
-    <hyperlink ref="F7" r:id="rId11" xr:uid="{BCF47F12-B47A-48D5-A310-25D2021910E3}"/>
-    <hyperlink ref="L7" r:id="rId12" xr:uid="{7DED0B92-4A5F-46D3-A600-BF2860882279}"/>
-    <hyperlink ref="F8" r:id="rId13" xr:uid="{0960048C-EAAB-4F3B-B98B-61023D8DC95C}"/>
-    <hyperlink ref="L8" r:id="rId14" xr:uid="{46D3BAE1-970B-4561-8E88-FA45E9F7E3F4}"/>
-    <hyperlink ref="F9" r:id="rId15" xr:uid="{BD1E913C-962A-4081-B1A6-4E38F6E41259}"/>
-    <hyperlink ref="L9" r:id="rId16" xr:uid="{2BEE5143-0D49-4029-83F7-AB52E83FDE5B}"/>
-    <hyperlink ref="F10" r:id="rId17" xr:uid="{E8FE4556-2258-4D94-B043-28EF6B6B0479}"/>
-    <hyperlink ref="L10" r:id="rId18" xr:uid="{1456CBFF-4E37-4573-A0FA-3FAFE8D4807E}"/>
-    <hyperlink ref="F11" r:id="rId19" xr:uid="{295C4CDE-2014-4799-837F-75F24C61B063}"/>
-    <hyperlink ref="L11" r:id="rId20" xr:uid="{D5947C03-F305-422F-8E2A-2EE6D66C7BA7}"/>
-    <hyperlink ref="F12" r:id="rId21" xr:uid="{4729A630-A9C8-45CF-A1C6-A1ACCCBF8FA9}"/>
-    <hyperlink ref="L12" r:id="rId22" xr:uid="{B9E6DF40-E054-42F2-B870-F93BE1CDD1EC}"/>
-    <hyperlink ref="F13" r:id="rId23" xr:uid="{E048198B-E4AF-4D7F-99CE-049A08846FE5}"/>
-    <hyperlink ref="L13" r:id="rId24" xr:uid="{14BE9966-146E-41C4-BD37-5F21883B5F9B}"/>
-    <hyperlink ref="F14" r:id="rId25" xr:uid="{9E1AD0BB-CBF2-4F35-9F4F-928CF6AD7DD1}"/>
-    <hyperlink ref="L14" r:id="rId26" xr:uid="{64C6AC31-B5BE-402A-A926-51B97FD41D36}"/>
-    <hyperlink ref="F15" r:id="rId27" xr:uid="{B59E4789-63DD-43D4-8B91-6FD68DBDE367}"/>
-    <hyperlink ref="L15" r:id="rId28" xr:uid="{55B14ACF-5C30-4D9B-90B8-BACAC04CC4C6}"/>
-    <hyperlink ref="F16" r:id="rId29" xr:uid="{12CD7407-F882-4649-958F-1F013216DD1A}"/>
-    <hyperlink ref="L16" r:id="rId30" xr:uid="{4B32E4BA-B970-4526-B4F2-119B4A21946C}"/>
-    <hyperlink ref="F17" r:id="rId31" xr:uid="{1AE9BD01-C175-4825-A336-39B57064047F}"/>
-    <hyperlink ref="L17" r:id="rId32" xr:uid="{9C8A8CEE-71F9-41D2-B491-96338CCDDB6D}"/>
-    <hyperlink ref="F18" r:id="rId33" xr:uid="{E45F13AE-BBE6-4C34-A6FB-D492E4736815}"/>
-    <hyperlink ref="L18" r:id="rId34" xr:uid="{B9A81F05-886B-4AAE-98D3-60AD282E4A8F}"/>
-    <hyperlink ref="F19" r:id="rId35" xr:uid="{1803C080-D2FE-4A6E-B098-EEE976CD16BB}"/>
-    <hyperlink ref="L19" r:id="rId36" xr:uid="{A532308F-DB0D-4BE5-90ED-606402367AAA}"/>
-    <hyperlink ref="F20" r:id="rId37" xr:uid="{9DFE5E21-3F2F-4374-BB56-AC638636F0AA}"/>
-    <hyperlink ref="L20" r:id="rId38" xr:uid="{3EA8B6D5-C002-45DC-8405-7F68EB775700}"/>
-    <hyperlink ref="F21" r:id="rId39" xr:uid="{5E23B10A-09D4-4C98-B5DA-FB8BACA5F226}"/>
-    <hyperlink ref="L21" r:id="rId40" xr:uid="{69938961-F60C-46C9-A9E0-4C4C78A60428}"/>
-    <hyperlink ref="F22" r:id="rId41" xr:uid="{024E2041-617C-4272-856A-CAF6C9F8EA0B}"/>
-    <hyperlink ref="L22" r:id="rId42" xr:uid="{AEA369BB-39B8-4D1F-8ED1-E7004649A6FD}"/>
-    <hyperlink ref="F23" r:id="rId43" xr:uid="{A8C2C4E8-803D-41B1-BCF6-9AAE35FE9461}"/>
-    <hyperlink ref="L23" r:id="rId44" xr:uid="{ECD31150-8418-4CDF-8818-7521D739BF1E}"/>
-    <hyperlink ref="F24" r:id="rId45" xr:uid="{4D1D7C0C-F3CC-4A79-9696-AE52AC49D818}"/>
-    <hyperlink ref="L24" r:id="rId46" xr:uid="{A27B4EEE-7FFB-4E7F-8E05-1C1B8C26D06C}"/>
-    <hyperlink ref="F25" r:id="rId47" xr:uid="{B0D0B877-D79A-46AC-ABEF-BD214D6A64DF}"/>
-    <hyperlink ref="L25" r:id="rId48" xr:uid="{B26384DA-D9B9-472E-8BCB-B8C3C703F256}"/>
-    <hyperlink ref="F26" r:id="rId49" xr:uid="{5A2F3502-5831-4322-A2A7-91AD9F0B7C1F}"/>
-    <hyperlink ref="L26" r:id="rId50" xr:uid="{677833C5-2A38-4551-AA52-D90C31259D8B}"/>
-    <hyperlink ref="F27" r:id="rId51" display="https://drive.google.com/file/d/1buDrBqk4rHcGLbKKMJHOEOM9AOosdrVF/view?usp=drive_link" xr:uid="{79967531-2A57-44D5-BD57-F0445E2D84E9}"/>
-    <hyperlink ref="L27" r:id="rId52" xr:uid="{745F3F22-C292-40E0-88A9-72DD1C6CDFCD}"/>
-    <hyperlink ref="F28" r:id="rId53" xr:uid="{4D8B81D2-7779-43DB-99C9-BB0976A21F9F}"/>
-    <hyperlink ref="L28" r:id="rId54" xr:uid="{9E7FF82C-9872-4F3A-A83F-710F7168E6BC}"/>
-    <hyperlink ref="F29" r:id="rId55" xr:uid="{E8A184F3-31F1-4D7B-81B0-154E96E9F503}"/>
-    <hyperlink ref="L29" r:id="rId56" xr:uid="{5271FFD9-D3C3-4391-B8F6-E21C7933B2BD}"/>
-    <hyperlink ref="F30" r:id="rId57" xr:uid="{FA16667E-68A4-47E5-9450-D7F6DB564A69}"/>
-    <hyperlink ref="L30" r:id="rId58" xr:uid="{D9A73594-AAE4-40F9-9D4A-C63F1AA4184A}"/>
-    <hyperlink ref="F31" r:id="rId59" xr:uid="{5BEA62FB-EFC3-4AB6-B8CD-9D1C6E0EDA0F}"/>
-    <hyperlink ref="L31" r:id="rId60" xr:uid="{95B2BB62-3B5E-4C9D-AF0E-5F455AEB6232}"/>
-    <hyperlink ref="F32" r:id="rId61" xr:uid="{4E8E792E-8744-4684-89E1-57D6C23E070C}"/>
-    <hyperlink ref="L32" r:id="rId62" xr:uid="{1D417491-01C3-4B03-A7DF-0ECACEA64C59}"/>
-    <hyperlink ref="F33" r:id="rId63" xr:uid="{9C1CAA25-A41A-4C4B-A04A-76D6487DE13E}"/>
-    <hyperlink ref="L33" r:id="rId64" xr:uid="{8F7477E3-8C4C-4ED7-9F06-4F39A668DC8B}"/>
-    <hyperlink ref="F34" r:id="rId65" xr:uid="{98332B7A-DE25-4C28-B854-B559E2CD1252}"/>
-    <hyperlink ref="L34" r:id="rId66" xr:uid="{DD1F7CFF-CB8C-4DE6-A118-5805173A893D}"/>
-    <hyperlink ref="F35" r:id="rId67" xr:uid="{948D2CBA-9336-403C-AA62-58EC637E9746}"/>
-    <hyperlink ref="L35" r:id="rId68" xr:uid="{B32D672A-4056-4235-882C-D4C84AEABD15}"/>
-    <hyperlink ref="F36" r:id="rId69" xr:uid="{85E4CCE6-F5CC-46DB-84CA-59E2229E2A2E}"/>
-    <hyperlink ref="L36" r:id="rId70" xr:uid="{8C070ED1-575B-41D9-BF9C-DD089A20FA71}"/>
-    <hyperlink ref="F37" r:id="rId71" xr:uid="{93252CD3-0380-4A84-B4DF-F38A391016A3}"/>
-    <hyperlink ref="L37" r:id="rId72" xr:uid="{7FDAAB39-303B-4095-8CF0-477946DBC3F1}"/>
-    <hyperlink ref="F38" r:id="rId73" xr:uid="{F05BA44A-4B1F-40D5-85F6-DAD064B8546F}"/>
-    <hyperlink ref="L38" r:id="rId74" xr:uid="{E5E89D99-8AC1-4914-9F6E-0259809EE6C7}"/>
-    <hyperlink ref="F39" r:id="rId75" xr:uid="{E1170239-2CC3-44D6-8EC7-0C2E5B080075}"/>
-    <hyperlink ref="L39" r:id="rId76" xr:uid="{BA5277F6-96B1-4827-8414-F1132F38E908}"/>
-    <hyperlink ref="F40" r:id="rId77" xr:uid="{B26364E6-F4C7-476E-A74F-B0058361AC71}"/>
-    <hyperlink ref="L40" r:id="rId78" xr:uid="{D50F68DC-7CAD-4162-BC38-240CBE904FFB}"/>
-    <hyperlink ref="F41" r:id="rId79" xr:uid="{3EB6F693-F4AE-44BD-A71C-7BC8880B9165}"/>
-    <hyperlink ref="L41" r:id="rId80" xr:uid="{FD3728E3-6372-4403-8C7B-77D2FACEFD15}"/>
-    <hyperlink ref="F42" r:id="rId81" xr:uid="{2DC1E206-159B-4E90-8A4D-00ED35EDF5FF}"/>
-    <hyperlink ref="F43" r:id="rId82" xr:uid="{603D8F37-9BF7-4960-99AE-8A310885D001}"/>
-    <hyperlink ref="L43" r:id="rId83" xr:uid="{BD9F1CF5-BF75-4E21-9533-79CF88B7A8C5}"/>
-    <hyperlink ref="F44" r:id="rId84" xr:uid="{2039E21D-E32C-49E0-B758-E6B72ED043ED}"/>
-    <hyperlink ref="L44" r:id="rId85" xr:uid="{8D39279B-E68B-4DC3-99BE-55D298339D6F}"/>
-    <hyperlink ref="F45" r:id="rId86" xr:uid="{F904DE0B-06ED-4BBF-AE9C-BD3958607565}"/>
-    <hyperlink ref="L45" r:id="rId87" xr:uid="{57396CEC-7B04-48D1-9DA4-4AC47DF9C6D9}"/>
-    <hyperlink ref="F46" r:id="rId88" xr:uid="{38AC5E9C-EF9E-4E99-B6C5-76DE1571FD87}"/>
-    <hyperlink ref="L46" r:id="rId89" xr:uid="{3193C4B6-EADD-4B64-B27E-0AEAB09CEC92}"/>
-    <hyperlink ref="F47" r:id="rId90" xr:uid="{0F6E0CBC-C1DB-4850-A9D8-6BC8F5DAD35F}"/>
-    <hyperlink ref="L47" r:id="rId91" xr:uid="{71413ED1-DA74-4C9B-9322-D408619CC0B4}"/>
-    <hyperlink ref="F48" r:id="rId92" xr:uid="{EF2382DD-D89C-486D-BC85-87F7ED5D46AA}"/>
-    <hyperlink ref="L48" r:id="rId93" xr:uid="{77A030EF-03A8-48EB-864E-CD30A6B974C6}"/>
-    <hyperlink ref="F49" r:id="rId94" xr:uid="{E4A958BF-662B-49BE-8933-75378FDC0D52}"/>
-    <hyperlink ref="L49" r:id="rId95" xr:uid="{0C8688AC-96E7-4286-9D4A-37A9996F4272}"/>
-    <hyperlink ref="F50" r:id="rId96" xr:uid="{12FED2CC-552A-4CF0-82A9-6228C6296899}"/>
-    <hyperlink ref="L50" r:id="rId97" xr:uid="{3CEEA9AD-1667-4186-9EF9-264886EE24C1}"/>
-    <hyperlink ref="F51" r:id="rId98" xr:uid="{EC43AB3E-1329-4317-BD37-E7F555F27326}"/>
-    <hyperlink ref="L51" r:id="rId99" xr:uid="{439DF3A7-37B3-4E22-9D93-A08BD9C64311}"/>
-    <hyperlink ref="F52" r:id="rId100" xr:uid="{E4890BFE-3BC3-42BC-B58B-303E4A0B694B}"/>
-    <hyperlink ref="L52" r:id="rId101" xr:uid="{4C755FDF-8D71-463A-9C66-13EA4042550E}"/>
-    <hyperlink ref="F53" r:id="rId102" xr:uid="{6637F6EC-7E0F-490A-8994-8AA645ABB08B}"/>
-    <hyperlink ref="L53" r:id="rId103" xr:uid="{787A0977-AE27-4F56-A9CF-4103F06E5EB2}"/>
-    <hyperlink ref="F54" r:id="rId104" xr:uid="{4321CCC7-36A7-4B52-9C7E-D20DBE6632B6}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{BF4871D9-1E6A-4FAB-86AC-B1CA162C2E6F}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{C693EA93-9F21-4ACE-8C74-C46F8B922D59}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{2599B7BE-C480-4166-83E1-8E8473E6C97E}"/>
+    <hyperlink ref="L3" r:id="rId4" xr:uid="{E485AC19-3BD8-4843-9F31-4AB755F96004}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{39314B55-4F5C-4126-9794-19DB324F0A2F}"/>
+    <hyperlink ref="L4" r:id="rId6" xr:uid="{EF0EE722-D4A0-4575-9243-61E64C2564A6}"/>
+    <hyperlink ref="F5" r:id="rId7" xr:uid="{54E80522-7BD2-4AFD-B34D-748F9946DEE3}"/>
+    <hyperlink ref="L5" r:id="rId8" xr:uid="{BA6ED292-98EF-4782-A5B4-96C5E748DD75}"/>
+    <hyperlink ref="F6" r:id="rId9" xr:uid="{0E903748-842D-4E69-903B-0E9F7D1124BC}"/>
+    <hyperlink ref="L6" r:id="rId10" xr:uid="{6A9E5D54-A0BD-43E6-ADCD-9F5E0CDFF719}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{0C04BAE9-4D85-4C9A-9CE9-C1EFBAE04A54}"/>
+    <hyperlink ref="L7" r:id="rId12" xr:uid="{11525ED1-4362-4E6A-8DED-F2E49F84DC39}"/>
+    <hyperlink ref="F8" r:id="rId13" xr:uid="{C2587CFA-A1DA-47BF-9FCF-9DC94AD8EF97}"/>
+    <hyperlink ref="L8" r:id="rId14" xr:uid="{0C4A514D-4E5C-4CFA-B3EB-12E4F53AD1DD}"/>
+    <hyperlink ref="F9" r:id="rId15" xr:uid="{A43558CA-55B2-4E53-AE7A-B77EEE86CC17}"/>
+    <hyperlink ref="L9" r:id="rId16" xr:uid="{BDD79251-CFB0-45B1-AE4F-3E8F41A47981}"/>
+    <hyperlink ref="F10" r:id="rId17" xr:uid="{C64D93EE-1B1A-4DA4-A1F3-D0985ACB7EC5}"/>
+    <hyperlink ref="L10" r:id="rId18" xr:uid="{99FC9A37-6115-46DE-A9A1-6A20326DBC3B}"/>
+    <hyperlink ref="F11" r:id="rId19" xr:uid="{50060AE3-3933-4595-B484-2A8219965D3F}"/>
+    <hyperlink ref="L11" r:id="rId20" xr:uid="{7EAA4FF2-BBE0-4073-8506-3B9ACC06D495}"/>
+    <hyperlink ref="F12" r:id="rId21" xr:uid="{4CB7CA0E-9CA0-402C-9657-27B218D63D45}"/>
+    <hyperlink ref="L12" r:id="rId22" xr:uid="{FC4F21B6-0DCF-4944-9AF8-39741E5C7C42}"/>
+    <hyperlink ref="F13" r:id="rId23" xr:uid="{D85FAC32-1BCD-40F7-A2CA-6B8E06C850DA}"/>
+    <hyperlink ref="L13" r:id="rId24" xr:uid="{88A981B4-CCF4-48C6-89F1-76F25009ED0A}"/>
+    <hyperlink ref="F14" r:id="rId25" xr:uid="{FFB2AB9E-271F-4E68-AC78-DB795A2108B5}"/>
+    <hyperlink ref="L14" r:id="rId26" xr:uid="{4D7EDD75-DC42-48B1-94CB-7924CB2A7CAE}"/>
+    <hyperlink ref="F15" r:id="rId27" xr:uid="{4DCB5AD4-4DBC-4C8B-82FD-A6B88673905F}"/>
+    <hyperlink ref="L15" r:id="rId28" xr:uid="{8426D3A1-7C0E-4DA6-82B3-42BA30D28CA1}"/>
+    <hyperlink ref="F16" r:id="rId29" xr:uid="{53CBAB83-A060-4897-A50A-75A6F90EFE9E}"/>
+    <hyperlink ref="L16" r:id="rId30" xr:uid="{EE3FAC74-04D0-4929-9FF9-B02266135527}"/>
+    <hyperlink ref="F17" r:id="rId31" xr:uid="{37E84704-02AC-4FC5-BEA8-20F7F067F293}"/>
+    <hyperlink ref="L17" r:id="rId32" xr:uid="{315EA7B0-1A62-48CB-8004-553F68A6825C}"/>
+    <hyperlink ref="F18" r:id="rId33" xr:uid="{4D31920F-4FFC-46FB-B311-702082CF266B}"/>
+    <hyperlink ref="L18" r:id="rId34" xr:uid="{832D894F-E975-4467-9F69-0D5C519CB8D7}"/>
+    <hyperlink ref="F19" r:id="rId35" xr:uid="{18E5557E-EB0A-42E7-824A-E63226208560}"/>
+    <hyperlink ref="L19" r:id="rId36" xr:uid="{D2914809-5099-46AA-9E8C-FA8517915020}"/>
+    <hyperlink ref="F20" r:id="rId37" xr:uid="{7A195B2D-D958-40C4-B50F-A1D1362E4C5C}"/>
+    <hyperlink ref="L20" r:id="rId38" xr:uid="{56000586-2E17-4688-ADA1-8B4C99693C03}"/>
+    <hyperlink ref="F21" r:id="rId39" xr:uid="{187CCA8F-56A0-443D-A257-2369B6E6FBEC}"/>
+    <hyperlink ref="L21" r:id="rId40" xr:uid="{5F3CC269-CFDB-41D2-A2F5-9575306E5C5F}"/>
+    <hyperlink ref="F22" r:id="rId41" xr:uid="{89B63224-36BA-4386-98CA-53BD6DEA785C}"/>
+    <hyperlink ref="L22" r:id="rId42" xr:uid="{070B3B55-B6DA-4D7D-96A1-0B38655B7EE5}"/>
+    <hyperlink ref="F23" r:id="rId43" xr:uid="{542656C7-0D07-48CB-BE60-C337D6B82BDE}"/>
+    <hyperlink ref="L23" r:id="rId44" xr:uid="{20DAC5B6-6C72-4C02-BBB5-39AB54DFE4FB}"/>
+    <hyperlink ref="F24" r:id="rId45" xr:uid="{F5B2BA3B-331A-480C-B1DC-D99A87AC3982}"/>
+    <hyperlink ref="L24" r:id="rId46" xr:uid="{D4802E10-61EC-4AEA-A21F-D48ACEE2AF4C}"/>
+    <hyperlink ref="F25" r:id="rId47" xr:uid="{F7AEB93C-57A8-4BEC-9309-9CCF86AEFD74}"/>
+    <hyperlink ref="L25" r:id="rId48" xr:uid="{569C8B00-05E5-4885-BC8C-23003D7FD7D1}"/>
+    <hyperlink ref="F26" r:id="rId49" xr:uid="{305146D1-D16B-423A-B9AE-64B61DB70208}"/>
+    <hyperlink ref="L26" r:id="rId50" xr:uid="{19BC3173-B2D0-44BF-96FD-D44F5780BE53}"/>
+    <hyperlink ref="F27" r:id="rId51" display="https://drive.google.com/file/d/1buDrBqk4rHcGLbKKMJHOEOM9AOosdrVF/view?usp=drive_link" xr:uid="{F2B92217-933B-40C6-9E0D-CDC57C3ABD25}"/>
+    <hyperlink ref="L27" r:id="rId52" xr:uid="{03D06138-3500-4731-882A-C37EC9194DB1}"/>
+    <hyperlink ref="F28" r:id="rId53" xr:uid="{09D61F21-63CF-4923-97B9-D6D685FCF725}"/>
+    <hyperlink ref="L28" r:id="rId54" xr:uid="{481922EA-C663-4FC4-B85B-1DF4F52A8D4D}"/>
+    <hyperlink ref="F29" r:id="rId55" xr:uid="{A447EEF4-C6FB-41A1-AC77-F823A2012E94}"/>
+    <hyperlink ref="L29" r:id="rId56" xr:uid="{B54BF329-7307-408A-9A08-09528434830A}"/>
+    <hyperlink ref="F30" r:id="rId57" xr:uid="{92D1FF1B-AAEF-4A86-95D3-E9EB523624AA}"/>
+    <hyperlink ref="L30" r:id="rId58" xr:uid="{516642FA-6318-4C35-B053-26827143CB59}"/>
+    <hyperlink ref="F31" r:id="rId59" xr:uid="{48E5B769-368A-4029-8C55-BB9E27DC42F4}"/>
+    <hyperlink ref="L31" r:id="rId60" xr:uid="{BE2A4988-4D0B-4EB4-BE11-17B0BD49DC8B}"/>
+    <hyperlink ref="F32" r:id="rId61" xr:uid="{A8B5CF5F-C59F-4A08-BE3E-0871678C66C9}"/>
+    <hyperlink ref="L32" r:id="rId62" xr:uid="{DE74A513-1010-487D-A1E5-C8B7528F48CB}"/>
+    <hyperlink ref="F33" r:id="rId63" xr:uid="{412368C3-1B36-401D-9645-A54DE65175EF}"/>
+    <hyperlink ref="L33" r:id="rId64" xr:uid="{6803A765-70D4-47D9-832E-061B4499C344}"/>
+    <hyperlink ref="F34" r:id="rId65" xr:uid="{5638778F-C664-43F9-A972-775A068EF781}"/>
+    <hyperlink ref="L34" r:id="rId66" xr:uid="{9328E37F-D22E-437B-8FC5-044D5624D77C}"/>
+    <hyperlink ref="F35" r:id="rId67" xr:uid="{67C6EDDE-DE10-4D5B-944C-5ED3E8EB1BA7}"/>
+    <hyperlink ref="L35" r:id="rId68" xr:uid="{985547D5-B505-4788-99A4-0154360F1A31}"/>
+    <hyperlink ref="F36" r:id="rId69" xr:uid="{1380A29E-FD2E-4CF5-9D4F-4AA31EEF3684}"/>
+    <hyperlink ref="L36" r:id="rId70" xr:uid="{2932EF15-ECB4-4970-A552-E41FDE73C11E}"/>
+    <hyperlink ref="F37" r:id="rId71" xr:uid="{DAC946FD-380B-47C2-8D73-216A770C0EEC}"/>
+    <hyperlink ref="L37" r:id="rId72" xr:uid="{444BDA33-DDBC-4270-9B2C-7333164ACC6F}"/>
+    <hyperlink ref="F38" r:id="rId73" xr:uid="{2199F9EC-6BE6-49EE-AB4A-5676605608ED}"/>
+    <hyperlink ref="L38" r:id="rId74" xr:uid="{0D6457B5-13A9-4B96-8725-EA526DC4CB5C}"/>
+    <hyperlink ref="F39" r:id="rId75" xr:uid="{1332CDD2-1C0B-4306-8363-658AC68E6398}"/>
+    <hyperlink ref="L39" r:id="rId76" xr:uid="{F05266ED-1994-4BE7-8222-6CAE1E20BA06}"/>
+    <hyperlink ref="F40" r:id="rId77" xr:uid="{5D7A7365-A8C5-49B3-9DF7-87FFEF7C2676}"/>
+    <hyperlink ref="L40" r:id="rId78" xr:uid="{96BC6402-59A6-4C40-9CA3-A7A93C8CDB0F}"/>
+    <hyperlink ref="F41" r:id="rId79" xr:uid="{A4D84D0C-311B-404B-B507-A9EF1D163EC7}"/>
+    <hyperlink ref="L41" r:id="rId80" xr:uid="{18F191BF-3EBD-447F-B12E-FB2E4F7716E7}"/>
+    <hyperlink ref="F42" r:id="rId81" xr:uid="{DB2CAA61-1D01-4EC3-8AFE-98D2A969DD40}"/>
+    <hyperlink ref="F43" r:id="rId82" xr:uid="{0FDEDDE5-3261-4C50-831C-6060A20FC48E}"/>
+    <hyperlink ref="L43" r:id="rId83" xr:uid="{EF0F958D-5A76-47A8-961C-26C91241A9F2}"/>
+    <hyperlink ref="F44" r:id="rId84" xr:uid="{2C6DD999-A8A8-42F1-A019-66AD6DC2175A}"/>
+    <hyperlink ref="L44" r:id="rId85" xr:uid="{55B780D0-7CB5-4062-9465-96E5CC3FD8E4}"/>
+    <hyperlink ref="F45" r:id="rId86" xr:uid="{7729B01B-5051-44C4-A9C8-70ACA5895AB9}"/>
+    <hyperlink ref="L45" r:id="rId87" xr:uid="{6D438157-69A3-4709-9BC6-8AC753B6558E}"/>
+    <hyperlink ref="F46" r:id="rId88" xr:uid="{83A0E19D-82F9-460E-8BCD-2C748D341B76}"/>
+    <hyperlink ref="L46" r:id="rId89" xr:uid="{5997857A-B084-470A-B7E8-3D1A3AEF0CEC}"/>
+    <hyperlink ref="F47" r:id="rId90" xr:uid="{AA21AF18-8995-4412-9DF0-0FC0B5459AA2}"/>
+    <hyperlink ref="L47" r:id="rId91" xr:uid="{51326B38-3A8B-44AC-A4A6-2CD88D23216F}"/>
+    <hyperlink ref="F48" r:id="rId92" xr:uid="{40C22073-A136-48B7-823D-D09A6D9A23D0}"/>
+    <hyperlink ref="L48" r:id="rId93" xr:uid="{783F25CC-FD28-4A2E-980B-77C1390D4064}"/>
+    <hyperlink ref="F49" r:id="rId94" xr:uid="{6F6BBF82-A1AA-4435-8C68-F2C94DBCC111}"/>
+    <hyperlink ref="L49" r:id="rId95" xr:uid="{84E89D86-034E-461E-8B2F-14A093498B6C}"/>
+    <hyperlink ref="F50" r:id="rId96" xr:uid="{B5A344BD-0991-4875-A8D1-1EF04C12A72A}"/>
+    <hyperlink ref="L50" r:id="rId97" xr:uid="{1325BE3D-68F1-4BFC-81E5-373DE57F1F16}"/>
+    <hyperlink ref="F51" r:id="rId98" xr:uid="{E2543043-AC62-4DCC-B2CE-83638B534A2A}"/>
+    <hyperlink ref="L51" r:id="rId99" xr:uid="{415A8DBF-67FE-4864-A8EF-EDC02192D9A5}"/>
+    <hyperlink ref="F52" r:id="rId100" xr:uid="{0F8A4830-596A-4547-BA5F-4B5570D631EC}"/>
+    <hyperlink ref="L52" r:id="rId101" xr:uid="{CEF0DFB0-AA13-4BFB-9C4C-0BDC8E75FAF4}"/>
+    <hyperlink ref="F53" r:id="rId102" xr:uid="{1D5FE741-48CD-4D14-9AA6-105873DB8366}"/>
+    <hyperlink ref="L53" r:id="rId103" xr:uid="{E8DF7D37-2642-4DBF-A8DA-FF792B416D9F}"/>
+    <hyperlink ref="F54" r:id="rId104" xr:uid="{E27549AE-23DF-4C8B-AE77-FC403C244CA2}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId105"/>

</xml_diff>